<commit_message>
Fixed intent DSL issue
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Application_JS.xlsx
@@ -421,18 +421,6 @@
     <t>Change Start page</t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-link_Click(Application_test_link);
-validate2;
-SelectTestToRun(VT281_0020_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(20);
-validate4;</t>
-  </si>
-  <si>
     <t>database file path with pre defined db partition "user"</t>
   </si>
   <si>
@@ -601,67 +589,6 @@
 };</t>
   </si>
   <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0031
-};
-validate4
-{
-validate_AppMinimized=Homescreen
-};
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0032
-};
-validate4
-{
-validate_AppMinimized=Appsscreen
-};
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0070
-};
-validate4
-{
-validate_PageTitle=Application JS Test
-};
-validate5
-{
-validate_AppMinimized=Homescreen
-};
-</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Manual specs
@@ -694,11 +621,11 @@
 };
 validate3
 {
-validate_Text_Exists=VT281-0077
+validate_Text_Exists=VT281-0078
 };
 validate4
 {
-validate_AppMinimized=AppsScreen
+validate_PageTitle=Application JS Test
 };
 validate5
 {
@@ -720,43 +647,9 @@
 };
 validate3
 {
-validate_Text_Exists=VT281-0078
+validate_Text_Exists=VT281-0080
 };
 validate4
-{
-validate_PageTitle=Application JS Test
-};
-validate5
-{
-validate_Result=UIDestroyed
-validate_Result=Deactivated
-validate_Result=Activated
-validate_doesNotContain=ScreenOff
-validate_doesNotContain=ScreenOn
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0079
-};
-validate4
-{
-validate_AppMinimized=AppsScreen
-};
-validate5
-{
-validate_PageTitle=Application JS Test
-};
-validate6
 {
 validate_Result=UIDestroyed
 validate_Result=Deactivated
@@ -766,7 +659,7 @@
 };</t>
   </si>
   <si>
-    <t>validate1
+    <t xml:space="preserve">validate1
 {
 validate_PageTitle=Manual specs
 };
@@ -776,97 +669,13 @@
 };
 validate3
 {
-validate_Text_Exists=VT281-0080
+validate_Text_Exists=VT281-0074
 };
 validate4
 {
-validate_Result=UIDestroyed
-validate_Result=Deactivated
-validate_Result=ScreenOff
-validate_Result=Activated
-validate_Result=ScreenOn
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0074
-};
-validate4
-{
 validate_Page=loadpage_xpath,Loading
 };
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0069
-};
-validate4
-{
-validate_Page=settingspage_xpath,Client ID
-};
-validate5
-{
-validate_PageTitle=Application JS Test
-};
-validate6
-{
-validate_Logdisplayed=LOG_TEST
-validate_Logdisplayed=menuCallback
-};
-validate7
-{
-validate_AppMinimized=Homescreen
-};
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT281-0007
-};
-validate5
-{
-validate_PageTitle=Manual specs
-};
-validate6
-{
-validate_PageTitle=Application JS Test
-};
-validate7
-{
-validate_Page=settingspage_xpath,Client ID
-};
-validate8
-{
-validate_AppMinimized=Homescreen
-};</t>
   </si>
   <si>
     <t>wait(3);
@@ -945,6 +754,197 @@
 ClickUITextView(Exit);
 validate7;
 </t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(Application_test_link);
+validate2;
+SelectTestToRun(VT281_0020_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(30);
+validate4;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0031
+};
+validate4
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0069
+};
+validate4
+{
+validate_Page=settingspage_xpath,Client ID
+};
+validate5
+{
+validate_PageTitle=Application JS Test
+};
+validate6
+{
+validate_Logdisplayed=LOG_TEST
+validate_Logdisplayed=menuCallback
+};
+validate7
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0070
+};
+validate4
+{
+validate_PageTitle=Application JS Test
+};
+validate5
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0032
+};
+validate4
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0077
+};
+validate4
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};
+validate5
+{
+validate_Result=UIDestroyed
+validate_Result=Deactivated
+validate_Result=Activated
+validate_doesNotContain=ScreenOff
+validate_doesNotContain=ScreenOn
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0079
+};
+validate4
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};
+validate5
+{
+validate_PageTitle=Application JS Test
+};
+validate6
+{
+validate_Result=UIDestroyed
+validate_Result=Deactivated
+validate_Result=ScreenOff
+validate_Result=Activated
+validate_Result=ScreenOn
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT281-0007
+};
+validate5
+{
+validate_PageTitle=Manual specs
+};
+validate6
+{
+validate_PageTitle=Application JS Test
+};
+validate7
+{
+validate_Page=settingspage_xpath,Client ID
+};
+validate8
+{
+validate_AppMinimized=com.symbol.enterprisebrowser
+};</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1425,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1501,7 +1501,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="370.5" thickBot="1">
+    <row r="3" spans="1:11" ht="383.25" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1519,10 +1519,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1549,7 +1549,7 @@
         <v>76</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1576,7 +1576,7 @@
         <v>77</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1600,10 +1600,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1630,7 +1630,7 @@
         <v>78</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1648,16 +1648,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1675,22 +1675,22 @@
         <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="217.5" thickBot="1">
+    <row r="10" spans="1:11" ht="230.25" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1711,13 +1711,13 @@
         <v>79</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="217.5" thickBot="1">
+    <row r="11" spans="1:11" ht="230.25" thickBot="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>80</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1760,16 +1760,16 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="11" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="294" thickBot="1">
+    <row r="13" spans="1:11" ht="306.75" thickBot="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1781,14 +1781,14 @@
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1815,7 +1815,7 @@
         <v>81</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1842,13 +1842,13 @@
         <v>82</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="306.75" thickBot="1">
+    <row r="16" spans="1:11" ht="319.5" thickBot="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1866,10 +1866,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1896,13 +1896,13 @@
         <v>83</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="357.75" thickBot="1">
+    <row r="18" spans="1:11" ht="370.5" thickBot="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>84</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1950,7 +1950,7 @@
         <v>85</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>

</xml_diff>

<commit_message>
Fixed automation gesture issues
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Application_JS.xlsx
@@ -472,14 +472,6 @@
 </t>
   </si>
   <si>
-    <t>wait(3);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
-ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
-ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Manual specs
@@ -945,6 +937,15 @@
 {
 validate_AppMinimized=com.symbol.enterprisebrowser
 };</t>
+  </si>
+  <si>
+    <t>wait(3);
+PullConfigxml;
+PullBkpConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
+PushConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1426,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1472,7 +1473,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="217.5" thickBot="1">
+    <row r="2" spans="1:11" ht="230.25" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1519,10 +1520,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1549,7 +1550,7 @@
         <v>76</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1576,7 +1577,7 @@
         <v>77</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1600,10 +1601,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1630,7 +1631,7 @@
         <v>78</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1657,7 +1658,7 @@
         <v>88</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1684,7 +1685,7 @@
         <v>89</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1711,7 +1712,7 @@
         <v>79</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1738,7 +1739,7 @@
         <v>80</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1760,10 +1761,10 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1788,7 +1789,7 @@
         <v>92</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1815,7 +1816,7 @@
         <v>81</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1842,7 +1843,7 @@
         <v>82</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1866,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1896,7 +1897,7 @@
         <v>83</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1923,7 +1924,7 @@
         <v>84</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1950,7 +1951,7 @@
         <v>85</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>

</xml_diff>